<commit_message>
created excel library for data extraction
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muzammil\OneDrive\Desktop\Projects\Testing Projects\PathologyLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400227B8-0508-4F30-9FBB-28F06E1EA2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDD06EA-98DB-4D0E-9344-ADA2E1A2E54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Testcases" sheetId="1" r:id="rId1"/>
+    <sheet name="Add test calculator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>SR.NO</t>
   </si>
@@ -79,12 +80,61 @@
   <si>
     <t>user not able to login and error message is displayed for incorrect password or username</t>
   </si>
+  <si>
+    <t>TC_CALCULATOR_01</t>
+  </si>
+  <si>
+    <t>Validate user is able to enter get estimate for tests successfully for test calculator in the site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. login with valid credentials
+2. enter test names 
+3. enter discount 
+4. validate subtotal and total Is matching or not
+</t>
+  </si>
+  <si>
+    <t>user is able to get estimate for tests successsfully</t>
+  </si>
+  <si>
+    <t>TC_CALCULATOR_01_DATA01</t>
+  </si>
+  <si>
+    <t>Select AFP test alpha feto proties test
+select 5% discount</t>
+  </si>
+  <si>
+    <t>TC_CALCUALTOR_02</t>
+  </si>
+  <si>
+    <t>VALIDATE SUBTOTAL AND TOTAL IS ZERO IF NOT TEST ARE SELECTED AND DISCOUNT IS SELECTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. login with valid credentials
+2. DO NOT ENTER TEST NAMES
+3. enter discount 
+4. validate subtotal and total Is matching or not
+</t>
+  </si>
+  <si>
+    <t>SUBTOTAL AND TOTAL AMOUNT SHOULD BE ZERO</t>
+  </si>
+  <si>
+    <t>TC_Calcualtor_02_01</t>
+  </si>
+  <si>
+    <t>select 5% discount</t>
+  </si>
+  <si>
+    <t>Select AFP test alpha feto proties test and VITAMIN B12
+select 5% discount</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +142,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +160,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,11 +203,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -423,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -498,4 +578,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5A7C85-8C69-4DDB-8A36-2B894ECD4C18}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="29.796875" customWidth="1"/>
+    <col min="3" max="3" width="42.19921875" customWidth="1"/>
+    <col min="4" max="4" width="21.796875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="24.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2.1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>